<commit_message>
Added protection to the report tab
to prevent accidental formula deletion.
</commit_message>
<xml_diff>
--- a/portfolio_dashboard_template.xlsx
+++ b/portfolio_dashboard_template.xlsx
@@ -13,19 +13,21 @@
     <sheet name="lists" sheetId="3" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Dashboard!$A$1:$N$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Dashboard!$A$1:$O$39</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Input!$A$1:$M$12</definedName>
     <definedName function="false" hidden="false" name="asset_classes" vbProcedure="false">lists!$A$1:$A$5</definedName>
     <definedName function="false" hidden="false" name="types" vbProcedure="false">lists!$D$1:$D$3</definedName>
     <definedName function="false" hidden="false" name="yesno" vbProcedure="false">lists!$G$1:$G$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Dashboard!$A$1:$O$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Dashboard!$A$1:$N$48</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Dashboard!$A$1:$O$39</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Dashboard!$A$1:$O$39</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">Dashboard!$A$1:$O$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">Dashboard!$A$1:$O$39</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Input!$A$1:$M$12</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">Input!$A$1:$M$12</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0" vbProcedure="false">Input!$A$1:$M$12</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">Input!$A$1:$M$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">Input!$A$1:$M$12</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -454,11 +456,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -467,23 +473,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -495,23 +501,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -519,15 +521,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -539,15 +541,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -559,19 +561,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -579,15 +581,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -595,19 +597,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -759,7 +753,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -804,8 +798,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.240797473723901"/>
-          <c:y val="0.0304752066115702"/>
+          <c:x val="0.240790986433663"/>
+          <c:y val="0.0304791424512463"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -843,10 +837,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0300230946882217"/>
-          <c:y val="0.212680785123967"/>
-          <c:w val="0.969788377244662"/>
-          <c:h val="0.786802685950413"/>
+          <c:x val="0.0300298919291791"/>
+          <c:y val="0.212708252615265"/>
+          <c:w val="0.969740170154058"/>
+          <c:h val="0.786646002841276"/>
         </c:manualLayout>
       </c:layout>
       <c:pie3DChart>
@@ -1045,7 +1039,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1091,8 +1085,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.626571091908877"/>
-          <c:y val="0.105282005371531"/>
+          <c:x val="0.62658349328215"/>
+          <c:y val="0.105300859598854"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1130,10 +1124,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0432050274941084"/>
-          <c:y val="0.0719785138764548"/>
-          <c:w val="0.544481539670071"/>
-          <c:h val="0.855147717099373"/>
+          <c:x val="0.0431861804222649"/>
+          <c:y val="0.0719914040114613"/>
+          <c:w val="0.544433781190019"/>
+          <c:h val="0.854942693409742"/>
         </c:manualLayout>
       </c:layout>
       <c:pie3DChart>
@@ -1318,6 +1312,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
+      <c:legendPos val="r"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
@@ -1326,6 +1321,7 @@
           <c:y val="0.571454154727794"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
           <a:srgbClr val="ffffff">
@@ -1352,7 +1348,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1398,8 +1394,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.644619329737377"/>
-          <c:y val="0.107000362713094"/>
+          <c:x val="0.644568965517241"/>
+          <c:y val="0.107019771449302"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1437,10 +1433,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0472190290918737"/>
-          <c:y val="0.0718171926006529"/>
-          <c:w val="0.544698912370678"/>
-          <c:h val="0.855096118969895"/>
+          <c:x val="0.0472413793103448"/>
+          <c:y val="0.0718302194812262"/>
+          <c:w val="0.544655172413793"/>
+          <c:h val="0.854888445492472"/>
         </c:manualLayout>
       </c:layout>
       <c:pie3DChart>
@@ -1625,6 +1621,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
+      <c:legendPos val="r"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
@@ -1633,6 +1630,7 @@
           <c:y val="0.449664429530201"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
           <a:srgbClr val="ffffff">
@@ -1670,9 +1668,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>92880</xdr:colOff>
+      <xdr:colOff>92520</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>58320</xdr:rowOff>
+      <xdr:rowOff>70560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1680,8 +1678,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5275440" y="262800"/>
-        <a:ext cx="7637760" cy="2787480"/>
+        <a:off x="5409000" y="262800"/>
+        <a:ext cx="7827840" cy="2787120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1696,13 +1694,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>16200</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>144360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>557640</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:colOff>557280</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>51120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1710,8 +1708,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5187960" y="3123720"/>
-        <a:ext cx="3665880" cy="2010240"/>
+        <a:off x="5321520" y="3123720"/>
+        <a:ext cx="3750840" cy="2009880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1726,13 +1724,13 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>498240</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>117360</xdr:rowOff>
+      <xdr:rowOff>129960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>45000</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>136080</xdr:rowOff>
+      <xdr:colOff>44640</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>11160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1740,8 +1738,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8794440" y="3109320"/>
-        <a:ext cx="4070880" cy="1984680"/>
+        <a:off x="9013320" y="3109320"/>
+        <a:ext cx="4175640" cy="1984320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1762,80 +1760,75 @@
   <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.6744186046512"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.9348837209302"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.6744186046512"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.8883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.2"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="10.093023255814"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-      <c r="L1" s="4" t="s">
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="5" t="n">
+      <c r="M1" s="6" t="n">
         <f aca="false">Input!C1</f>
         <v>42748</v>
       </c>
-      <c r="N1" s="5"/>
-    </row>
-    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="10" t="n">
+      <c r="B5" s="2" t="n">
         <f aca="false">Input!C30</f>
         <v>0</v>
       </c>
-      <c r="C5" s="1" t="e">
+      <c r="C5" s="2" t="e">
         <f aca="false">E5/SUM(Input!$H$4:$H$79)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1870,14 +1863,14 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="10" t="n">
+      <c r="B7" s="2" t="n">
         <f aca="false">Input!C32</f>
         <v>0</v>
       </c>
-      <c r="C7" s="1" t="e">
+      <c r="C7" s="2" t="e">
         <f aca="false">E7/SUM(Input!$H$4:$H$79)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1912,14 +1905,14 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="10" t="n">
+      <c r="B9" s="2" t="n">
         <f aca="false">Input!C34</f>
         <v>0</v>
       </c>
-      <c r="C9" s="1" t="e">
+      <c r="C9" s="2" t="e">
         <f aca="false">E9/SUM(Input!$H$4:$H$79)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1944,49 +1937,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0"/>
-      <c r="C11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+    <row r="11" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="10" t="n">
+      <c r="B14" s="2" t="n">
         <f aca="false">(Input!C39)</f>
         <v>0</v>
       </c>
-      <c r="C14" s="10" t="e">
+      <c r="C14" s="2" t="e">
         <f aca="false">E14/$E$19</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D14" s="10" t="e">
+      <c r="D14" s="2" t="e">
         <f aca="false">C14-B14</f>
         <v>#DIV/0!</v>
       </c>
@@ -2017,18 +2007,18 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="10" t="n">
+      <c r="B16" s="2" t="n">
         <f aca="false">(Input!C41)</f>
         <v>0</v>
       </c>
-      <c r="C16" s="10" t="e">
+      <c r="C16" s="2" t="e">
         <f aca="false">E16/$E$19</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D16" s="10" t="e">
+      <c r="D16" s="2" t="e">
         <f aca="false">C16-B16</f>
         <v>#DIV/0!</v>
       </c>
@@ -2059,18 +2049,18 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="10" t="n">
+      <c r="B18" s="2" t="n">
         <f aca="false">(Input!C43)</f>
         <v>0</v>
       </c>
-      <c r="C18" s="10" t="e">
+      <c r="C18" s="2" t="e">
         <f aca="false">E18/$E$19</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D18" s="10" t="e">
+      <c r="D18" s="2" t="e">
         <f aca="false">C18-B18</f>
         <v>#DIV/0!</v>
       </c>
@@ -2079,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="s">
         <v>13</v>
       </c>
@@ -2091,49 +2081,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0"/>
-      <c r="C20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
+    <row r="20" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="s">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="10" t="n">
+      <c r="B23" s="2" t="n">
         <f aca="false">Input!C48</f>
         <v>0</v>
       </c>
-      <c r="C23" s="10" t="e">
+      <c r="C23" s="2" t="e">
         <f aca="false">E23/$E$28</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D23" s="10" t="e">
+      <c r="D23" s="2" t="e">
         <f aca="false">C23-B23</f>
         <v>#DIV/0!</v>
       </c>
@@ -2164,18 +2151,18 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="10" t="n">
+      <c r="B25" s="2" t="n">
         <f aca="false">Input!C50</f>
         <v>0</v>
       </c>
-      <c r="C25" s="10" t="e">
+      <c r="C25" s="2" t="e">
         <f aca="false">E25/$E$28</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D25" s="10" t="e">
+      <c r="D25" s="2" t="e">
         <f aca="false">C25-B25</f>
         <v>#DIV/0!</v>
       </c>
@@ -2206,18 +2193,18 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="10" t="n">
+      <c r="B27" s="2" t="n">
         <f aca="false">Input!C52</f>
         <v>0</v>
       </c>
-      <c r="C27" s="10" t="e">
+      <c r="C27" s="2" t="e">
         <f aca="false">E27/$E$28</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D27" s="10" t="e">
+      <c r="D27" s="2" t="e">
         <f aca="false">C27-B27</f>
         <v>#DIV/0!</v>
       </c>
@@ -2226,7 +2213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="18" t="s">
         <v>13</v>
       </c>
@@ -2238,20 +2225,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0"/>
-      <c r="C29" s="0"/>
-    </row>
-    <row r="30" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0"/>
-      <c r="C30" s="0"/>
-    </row>
-    <row r="31" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
+    <row r="29" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" s="1" customFormat="true" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="0"/>
-      <c r="C31" s="0"/>
       <c r="J31" s="22" t="s">
         <v>17</v>
       </c>
@@ -2979,6 +2958,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <mergeCells count="5">
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="A3:E3"/>
@@ -3005,854 +2985,911 @@
   <dimension ref="A1:R52"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="18.8279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="35" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="35" width="52.9162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="35" width="21.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="35" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="36" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="36" width="15.8744186046512"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="37" width="12.553488372093"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="37" width="13.5348837209302"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="37" width="9.47441860465116"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="37" width="15.506976744186"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="37" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="35" width="12.6744186046512"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="35" width="12.9209302325581"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="35" width="12.6744186046512"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="35" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="35" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="35" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.4418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="54.3953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.5348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="35" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="35" width="16.246511627907"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="36" width="12.8"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="36" width="13.906976744186"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="36" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="36" width="15.8744186046512"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="36" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="10.093023255814"/>
   </cols>
   <sheetData>
-    <row r="1" s="35" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="38" t="s">
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="39" t="n">
+      <c r="B1" s="4"/>
+      <c r="C1" s="37" t="n">
         <v>42748</v>
       </c>
     </row>
-    <row r="2" s="35" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I2" s="40" t="s">
+    <row r="2" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0"/>
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
+      <c r="I2" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="0"/>
+      <c r="O2" s="0"/>
+      <c r="P2" s="0"/>
+      <c r="Q2" s="0"/>
+      <c r="R2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="43" t="s">
+      <c r="I3" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="43" t="s">
+      <c r="J3" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="43" t="s">
+      <c r="L3" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="44" t="s">
+      <c r="M3" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="38" t="s">
+      <c r="N3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="38" t="s">
+      <c r="O3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="P3" s="38" t="s">
+      <c r="P3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Q3" s="38" t="s">
+      <c r="Q3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="R3" s="38" t="s">
+      <c r="R3" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47" t="n">
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="45" t="n">
         <f aca="false">F4*G4</f>
         <v>0</v>
       </c>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="49" t="n">
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="47" t="n">
         <f aca="false">I4*$H4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="49" t="n">
+      <c r="O4" s="47" t="n">
         <f aca="false">J4*$H4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="49" t="n">
+      <c r="P4" s="47" t="n">
         <f aca="false">K4*$H4</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="49" t="n">
+      <c r="Q4" s="47" t="n">
         <f aca="false">L4*$H4</f>
         <v>0</v>
       </c>
-      <c r="R4" s="49" t="n">
+      <c r="R4" s="47" t="n">
         <f aca="false">M4*$H4</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="45"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="47" t="n">
+      <c r="A5" s="43"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="45" t="n">
         <f aca="false">F5*G5</f>
         <v>0</v>
       </c>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="49" t="n">
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="47" t="n">
         <f aca="false">I5*$H5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="49" t="n">
+      <c r="O5" s="47" t="n">
         <f aca="false">J5*$H5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="49" t="n">
+      <c r="P5" s="47" t="n">
         <f aca="false">K5*$H5</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="49" t="n">
+      <c r="Q5" s="47" t="n">
         <f aca="false">L5*$H5</f>
         <v>0</v>
       </c>
-      <c r="R5" s="49" t="n">
+      <c r="R5" s="47" t="n">
         <f aca="false">M5*$H5</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="45"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="47" t="n">
+      <c r="A6" s="43"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="45" t="n">
         <f aca="false">F6*G6</f>
         <v>0</v>
       </c>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="49" t="n">
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="47" t="n">
         <f aca="false">I6*$H6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="49" t="n">
+      <c r="O6" s="47" t="n">
         <f aca="false">J6*$H6</f>
         <v>0</v>
       </c>
-      <c r="P6" s="49" t="n">
+      <c r="P6" s="47" t="n">
         <f aca="false">K6*$H6</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="49" t="n">
+      <c r="Q6" s="47" t="n">
         <f aca="false">L6*$H6</f>
         <v>0</v>
       </c>
-      <c r="R6" s="49" t="n">
+      <c r="R6" s="47" t="n">
         <f aca="false">M6*$H6</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="45"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="47" t="n">
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="45" t="n">
         <f aca="false">F7*G7</f>
         <v>0</v>
       </c>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="49" t="n">
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="47" t="n">
         <f aca="false">I7*$H7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="49" t="n">
+      <c r="O7" s="47" t="n">
         <f aca="false">J7*$H7</f>
         <v>0</v>
       </c>
-      <c r="P7" s="49" t="n">
+      <c r="P7" s="47" t="n">
         <f aca="false">K7*$H7</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="49" t="n">
+      <c r="Q7" s="47" t="n">
         <f aca="false">L7*$H7</f>
         <v>0</v>
       </c>
-      <c r="R7" s="49" t="n">
+      <c r="R7" s="47" t="n">
         <f aca="false">M7*$H7</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="45"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="47" t="n">
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="45" t="n">
         <f aca="false">F8*G8</f>
         <v>0</v>
       </c>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="49" t="n">
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="47" t="n">
         <f aca="false">I8*$H8</f>
         <v>0</v>
       </c>
-      <c r="O8" s="49" t="n">
+      <c r="O8" s="47" t="n">
         <f aca="false">J8*$H8</f>
         <v>0</v>
       </c>
-      <c r="P8" s="49" t="n">
+      <c r="P8" s="47" t="n">
         <f aca="false">K8*$H8</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="49" t="n">
+      <c r="Q8" s="47" t="n">
         <f aca="false">L8*$H8</f>
         <v>0</v>
       </c>
-      <c r="R8" s="49" t="n">
+      <c r="R8" s="47" t="n">
         <f aca="false">M8*$H8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="45"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="47" t="n">
+      <c r="A9" s="43"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="45" t="n">
         <f aca="false">F9*G9</f>
         <v>0</v>
       </c>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="49" t="n">
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="47" t="n">
         <f aca="false">I9*$H9</f>
         <v>0</v>
       </c>
-      <c r="O9" s="49" t="n">
+      <c r="O9" s="47" t="n">
         <f aca="false">J9*$H9</f>
         <v>0</v>
       </c>
-      <c r="P9" s="49" t="n">
+      <c r="P9" s="47" t="n">
         <f aca="false">K9*$H9</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="49" t="n">
+      <c r="Q9" s="47" t="n">
         <f aca="false">L9*$H9</f>
         <v>0</v>
       </c>
-      <c r="R9" s="49" t="n">
+      <c r="R9" s="47" t="n">
         <f aca="false">M9*$H9</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="45"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="47" t="n">
+      <c r="A10" s="43"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="45" t="n">
         <f aca="false">F10*G10</f>
         <v>0</v>
       </c>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="49" t="n">
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="47" t="n">
         <f aca="false">I10*$H10</f>
         <v>0</v>
       </c>
-      <c r="O10" s="49" t="n">
+      <c r="O10" s="47" t="n">
         <f aca="false">J10*$H10</f>
         <v>0</v>
       </c>
-      <c r="P10" s="49" t="n">
+      <c r="P10" s="47" t="n">
         <f aca="false">K10*$H10</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="49" t="n">
+      <c r="Q10" s="47" t="n">
         <f aca="false">L10*$H10</f>
         <v>0</v>
       </c>
-      <c r="R10" s="49" t="n">
+      <c r="R10" s="47" t="n">
         <f aca="false">M10*$H10</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="45"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="47" t="n">
+      <c r="A11" s="43"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="45" t="n">
         <f aca="false">F11*G11</f>
         <v>0</v>
       </c>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="49" t="n">
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="47" t="n">
         <f aca="false">I11*$H11</f>
         <v>0</v>
       </c>
-      <c r="O11" s="49" t="n">
+      <c r="O11" s="47" t="n">
         <f aca="false">J11*$H11</f>
         <v>0</v>
       </c>
-      <c r="P11" s="49" t="n">
+      <c r="P11" s="47" t="n">
         <f aca="false">K11*$H11</f>
         <v>0</v>
       </c>
-      <c r="Q11" s="49" t="n">
+      <c r="Q11" s="47" t="n">
         <f aca="false">L11*$H11</f>
         <v>0</v>
       </c>
-      <c r="R11" s="49" t="n">
+      <c r="R11" s="47" t="n">
         <f aca="false">M11*$H11</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="45"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="47" t="n">
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="45" t="n">
         <f aca="false">F12*G12</f>
         <v>0</v>
       </c>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="49" t="n">
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="47" t="n">
         <f aca="false">I12*$H12</f>
         <v>0</v>
       </c>
-      <c r="O12" s="49" t="n">
+      <c r="O12" s="47" t="n">
         <f aca="false">J12*$H12</f>
         <v>0</v>
       </c>
-      <c r="P12" s="49" t="n">
+      <c r="P12" s="47" t="n">
         <f aca="false">K12*$H12</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="49" t="n">
+      <c r="Q12" s="47" t="n">
         <f aca="false">L12*$H12</f>
         <v>0</v>
       </c>
-      <c r="R12" s="49" t="n">
+      <c r="R12" s="47" t="n">
         <f aca="false">M12*$H12</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="45"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="47" t="n">
+      <c r="A13" s="43"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="45" t="n">
         <f aca="false">F13*G13</f>
         <v>0</v>
       </c>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="49" t="n">
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="47" t="n">
         <f aca="false">I13*$H13</f>
         <v>0</v>
       </c>
-      <c r="O13" s="49" t="n">
+      <c r="O13" s="47" t="n">
         <f aca="false">J13*$H13</f>
         <v>0</v>
       </c>
-      <c r="P13" s="49" t="n">
+      <c r="P13" s="47" t="n">
         <f aca="false">K13*$H13</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="49" t="n">
+      <c r="Q13" s="47" t="n">
         <f aca="false">L13*$H13</f>
         <v>0</v>
       </c>
-      <c r="R13" s="49" t="n">
+      <c r="R13" s="47" t="n">
         <f aca="false">M13*$H13</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="45"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="47" t="n">
+      <c r="A14" s="43"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="45" t="n">
         <f aca="false">F14*G14</f>
         <v>0</v>
       </c>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="49" t="n">
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="47" t="n">
         <f aca="false">I14*$H14</f>
         <v>0</v>
       </c>
-      <c r="O14" s="49" t="n">
+      <c r="O14" s="47" t="n">
         <f aca="false">J14*$H14</f>
         <v>0</v>
       </c>
-      <c r="P14" s="49" t="n">
+      <c r="P14" s="47" t="n">
         <f aca="false">K14*$H14</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="49" t="n">
+      <c r="Q14" s="47" t="n">
         <f aca="false">L14*$H14</f>
         <v>0</v>
       </c>
-      <c r="R14" s="49" t="n">
+      <c r="R14" s="47" t="n">
         <f aca="false">M14*$H14</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="45"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="47" t="n">
+      <c r="A15" s="43"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="45" t="n">
         <f aca="false">F15*G15</f>
         <v>0</v>
       </c>
-      <c r="I15" s="48"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="49" t="n">
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="47" t="n">
         <f aca="false">I15*$H15</f>
         <v>0</v>
       </c>
-      <c r="O15" s="49" t="n">
+      <c r="O15" s="47" t="n">
         <f aca="false">J15*$H15</f>
         <v>0</v>
       </c>
-      <c r="P15" s="49" t="n">
+      <c r="P15" s="47" t="n">
         <f aca="false">K15*$H15</f>
         <v>0</v>
       </c>
-      <c r="Q15" s="49" t="n">
+      <c r="Q15" s="47" t="n">
         <f aca="false">L15*$H15</f>
         <v>0</v>
       </c>
-      <c r="R15" s="49" t="n">
+      <c r="R15" s="47" t="n">
         <f aca="false">M15*$H15</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="45"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="47" t="n">
+      <c r="A16" s="43"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="45" t="n">
         <f aca="false">F16*G16</f>
         <v>0</v>
       </c>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="48"/>
-      <c r="L16" s="48"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="49" t="n">
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="46"/>
+      <c r="N16" s="47" t="n">
         <f aca="false">I16*$H16</f>
         <v>0</v>
       </c>
-      <c r="O16" s="49" t="n">
+      <c r="O16" s="47" t="n">
         <f aca="false">J16*$H16</f>
         <v>0</v>
       </c>
-      <c r="P16" s="49" t="n">
+      <c r="P16" s="47" t="n">
         <f aca="false">K16*$H16</f>
         <v>0</v>
       </c>
-      <c r="Q16" s="49" t="n">
+      <c r="Q16" s="47" t="n">
         <f aca="false">L16*$H16</f>
         <v>0</v>
       </c>
-      <c r="R16" s="49" t="n">
+      <c r="R16" s="47" t="n">
         <f aca="false">M16*$H16</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="45"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="47" t="n">
+      <c r="A17" s="43"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="45" t="n">
         <f aca="false">F17*G17</f>
         <v>0</v>
       </c>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="49" t="n">
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="47" t="n">
         <f aca="false">I17*$H17</f>
         <v>0</v>
       </c>
-      <c r="O17" s="49" t="n">
+      <c r="O17" s="47" t="n">
         <f aca="false">J17*$H17</f>
         <v>0</v>
       </c>
-      <c r="P17" s="49" t="n">
+      <c r="P17" s="47" t="n">
         <f aca="false">K17*$H17</f>
         <v>0</v>
       </c>
-      <c r="Q17" s="49" t="n">
+      <c r="Q17" s="47" t="n">
         <f aca="false">L17*$H17</f>
         <v>0</v>
       </c>
-      <c r="R17" s="49" t="n">
+      <c r="R17" s="47" t="n">
         <f aca="false">M17*$H17</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="45"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="47" t="n">
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="45" t="n">
         <f aca="false">F18*G18</f>
         <v>0</v>
       </c>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="49" t="n">
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="47" t="n">
         <f aca="false">I18*$H18</f>
         <v>0</v>
       </c>
-      <c r="O18" s="49" t="n">
+      <c r="O18" s="47" t="n">
         <f aca="false">J18*$H18</f>
         <v>0</v>
       </c>
-      <c r="P18" s="49" t="n">
+      <c r="P18" s="47" t="n">
         <f aca="false">K18*$H18</f>
         <v>0</v>
       </c>
-      <c r="Q18" s="49" t="n">
+      <c r="Q18" s="47" t="n">
         <f aca="false">L18*$H18</f>
         <v>0</v>
       </c>
-      <c r="R18" s="49" t="n">
+      <c r="R18" s="47" t="n">
         <f aca="false">M18*$H18</f>
         <v>0</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+    </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="50"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
+      <c r="A21" s="48"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0"/>
+      <c r="B22" s="0"/>
+      <c r="C22" s="0"/>
+      <c r="D22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0"/>
+      <c r="B24" s="0"/>
+      <c r="C24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0"/>
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0"/>
+      <c r="B27" s="0"/>
+      <c r="C27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="52" t="s">
+      <c r="A28" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="52"/>
-      <c r="C28" s="52"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="53" t="s">
+      <c r="A29" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="53"/>
-      <c r="C29" s="54" t="s">
+      <c r="B29" s="51"/>
+      <c r="C29" s="52" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="55" t="s">
+      <c r="A30" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="55"/>
-      <c r="C30" s="48"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="46"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="48"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="46"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="55" t="s">
+      <c r="A32" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="55"/>
-      <c r="C32" s="48"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="46"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="56" t="s">
+      <c r="A33" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="56"/>
-      <c r="C33" s="48"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="46"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="57" t="s">
+      <c r="A34" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="57"/>
-      <c r="C34" s="48"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="46"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0"/>
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0"/>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="51" t="s">
+      <c r="A37" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="51"/>
-      <c r="C37" s="51"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="53"/>
-      <c r="C38" s="54" t="s">
+      <c r="B38" s="51"/>
+      <c r="C38" s="52" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="55" t="s">
+      <c r="A39" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="55"/>
-      <c r="C39" s="48"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="46"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="56" t="s">
+      <c r="A40" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B40" s="56"/>
-      <c r="C40" s="48"/>
+      <c r="B40" s="54"/>
+      <c r="C40" s="46"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="55" t="s">
+      <c r="A41" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="55"/>
-      <c r="C41" s="48"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="46"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="56" t="s">
+      <c r="A42" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="48"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="46"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="57" t="s">
+      <c r="A43" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="57"/>
-      <c r="C43" s="48"/>
+      <c r="B43" s="55"/>
+      <c r="C43" s="46"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0"/>
+      <c r="B44" s="0"/>
+      <c r="C44" s="0"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0"/>
+      <c r="B45" s="0"/>
+      <c r="C45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="51" t="s">
+      <c r="A46" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="51"/>
-      <c r="C46" s="51"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="49"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="53" t="s">
+      <c r="A47" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="53"/>
-      <c r="C47" s="54" t="s">
+      <c r="B47" s="51"/>
+      <c r="C47" s="52" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="55" t="s">
+      <c r="A48" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B48" s="55"/>
-      <c r="C48" s="48"/>
+      <c r="B48" s="53"/>
+      <c r="C48" s="46"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="56" t="s">
+      <c r="A49" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B49" s="56"/>
-      <c r="C49" s="48"/>
+      <c r="B49" s="54"/>
+      <c r="C49" s="46"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="55" t="s">
+      <c r="A50" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="55"/>
-      <c r="C50" s="48"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="46"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="56" t="s">
+      <c r="A51" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B51" s="56"/>
-      <c r="C51" s="48"/>
+      <c r="B51" s="54"/>
+      <c r="C51" s="46"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="57" t="s">
+      <c r="A52" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B52" s="57"/>
-      <c r="C52" s="48"/>
+      <c r="B52" s="55"/>
+      <c r="C52" s="46"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true"/>
@@ -3941,7 +3978,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5023255813953"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>